<commit_message>
OPSK-1660 new base template with embedded rightfield logo
</commit_message>
<xml_diff>
--- a/config/default_data/base-samples-template.xlsx
+++ b/config/default_data/base-samples-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20685" windowHeight="10995" tabRatio="992"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="290">
   <si>
     <t>Experimental_assay_type</t>
   </si>
@@ -912,6 +912,9 @@
   </si>
   <si>
     <t>SOP SEEK ID:</t>
+  </si>
+  <si>
+    <t>Powered by:</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1167,6 +1170,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1367,6 +1373,52 @@
         </a:ln>
       </xdr:spPr>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>494055</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571695</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>209098</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10299202" y="4347882"/>
+          <a:ext cx="1511993" cy="399598"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1662,7 +1714,7 @@
   <dimension ref="A2:AMJ19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1681,50 +1733,50 @@
         <v>280</v>
       </c>
       <c r="C2" s="11"/>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
       <c r="C3" s="12"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="29"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>275</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29"/>
-    </row>
-    <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="30"/>
+    </row>
+    <row r="5" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
         <v>276</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="29"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
@@ -1733,24 +1785,24 @@
       <c r="C6" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="29"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="31" t="s">
         <v>282</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
@@ -1830,21 +1882,24 @@
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+    <row r="16" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="24" t="s">
         <v>285</v>
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="2:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>286</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
         <v>287</v>
       </c>
@@ -1852,7 +1907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>288</v>
       </c>

</xml_diff>